<commit_message>
Fix drug code link format
</commit_message>
<xml_diff>
--- a/check_links/summary_data.xlsx
+++ b/check_links/summary_data.xlsx
@@ -13127,17 +13127,17 @@
     <row r="748">
       <c r="A748" t="inlineStr">
         <is>
-          <t>Amino Acids (Essential &amp; Nonessential )</t>
+          <t>Amino Acids</t>
         </is>
       </c>
       <c r="B748" t="inlineStr">
         <is>
-          <t>amino-acids-(essential-&amp;-nonessential-)</t>
+          <t>amino-acids</t>
         </is>
       </c>
       <c r="C748" t="inlineStr">
         <is>
-          <t>[UpToDate](https://www.uptodate.com/contents/amino-acids-(essential-&amp;-nonessential-)-drug-information)</t>
+          <t>[UpToDate](https://www.uptodate.com/contents/amino-acids-drug-information)</t>
         </is>
       </c>
     </row>

</xml_diff>